<commit_message>
alterações na estrutura e outras atualizações
</commit_message>
<xml_diff>
--- a/form4/V2_belem_atualizado_form4.xlsx
+++ b/form4/V2_belem_atualizado_form4.xlsx
@@ -56,7 +56,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
@@ -71,8 +71,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF6666"/>
-        <bgColor rgb="00FF6666"/>
+        <fgColor rgb="0066FF66"/>
+        <bgColor rgb="0066FF66"/>
       </patternFill>
     </fill>
     <fill>
@@ -89,8 +89,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00FF6666"/>
+        <bgColor rgb="00FF6666"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00A020F0"/>
         <bgColor rgb="00A020F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF6400"/>
+        <bgColor rgb="00FF6400"/>
       </patternFill>
     </fill>
   </fills>
@@ -120,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -137,7 +149,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -614,7 +632,7 @@
       </c>
       <c r="G2" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="H2" s="3" t="n"/>
@@ -657,7 +675,7 @@
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="H3" s="3" t="n"/>
@@ -700,7 +718,7 @@
       </c>
       <c r="G4" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="H4" s="3" t="n"/>
@@ -743,7 +761,7 @@
       </c>
       <c r="G5" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="H5" s="3" t="n"/>
@@ -865,7 +883,7 @@
       </c>
       <c r="E2" s="3" t="n"/>
       <c r="F2" s="3" t="n"/>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -900,7 +918,7 @@
       </c>
       <c r="E3" s="3" t="n"/>
       <c r="F3" s="3" t="n"/>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -935,7 +953,7 @@
       </c>
       <c r="E4" s="3" t="n"/>
       <c r="F4" s="3" t="n"/>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -970,7 +988,7 @@
       </c>
       <c r="E5" s="3" t="n"/>
       <c r="F5" s="3" t="n"/>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1094,7 +1112,7 @@
       </c>
       <c r="E2" s="3" t="n"/>
       <c r="F2" s="3" t="n"/>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1129,7 +1147,7 @@
       </c>
       <c r="E3" s="3" t="n"/>
       <c r="F3" s="3" t="n"/>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1164,7 +1182,7 @@
       </c>
       <c r="E4" s="3" t="n"/>
       <c r="F4" s="3" t="n"/>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1199,7 +1217,7 @@
       </c>
       <c r="E5" s="3" t="n"/>
       <c r="F5" s="3" t="n"/>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1323,7 +1341,7 @@
       </c>
       <c r="E2" s="3" t="n"/>
       <c r="F2" s="3" t="n"/>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1358,7 +1376,7 @@
       </c>
       <c r="E3" s="3" t="n"/>
       <c r="F3" s="3" t="n"/>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1393,7 +1411,7 @@
       </c>
       <c r="E4" s="3" t="n"/>
       <c r="F4" s="3" t="n"/>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1428,7 +1446,7 @@
       </c>
       <c r="E5" s="3" t="n"/>
       <c r="F5" s="3" t="n"/>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1552,7 +1570,7 @@
       </c>
       <c r="E2" s="3" t="n"/>
       <c r="F2" s="3" t="n"/>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1587,7 +1605,7 @@
       </c>
       <c r="E3" s="3" t="n"/>
       <c r="F3" s="3" t="n"/>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1622,7 +1640,7 @@
       </c>
       <c r="E4" s="3" t="n"/>
       <c r="F4" s="3" t="n"/>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1657,7 +1675,7 @@
       </c>
       <c r="E5" s="3" t="n"/>
       <c r="F5" s="3" t="n"/>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1781,7 +1799,7 @@
       </c>
       <c r="E2" s="3" t="n"/>
       <c r="F2" s="3" t="n"/>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1816,7 +1834,7 @@
       </c>
       <c r="E3" s="3" t="n"/>
       <c r="F3" s="3" t="n"/>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1851,7 +1869,7 @@
       </c>
       <c r="E4" s="3" t="n"/>
       <c r="F4" s="3" t="n"/>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -1886,7 +1904,7 @@
       </c>
       <c r="E5" s="3" t="n"/>
       <c r="F5" s="3" t="n"/>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -2150,7 +2168,7 @@
       </c>
       <c r="G2" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="H2" s="3" t="n"/>
@@ -2193,7 +2211,7 @@
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="H3" s="3" t="n"/>
@@ -2236,7 +2254,7 @@
       </c>
       <c r="G4" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="H4" s="3" t="n"/>
@@ -2279,7 +2297,7 @@
       </c>
       <c r="G5" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="H5" s="3" t="n"/>
@@ -2411,7 +2429,7 @@
       </c>
       <c r="G2" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="H2" s="3" t="n"/>
@@ -2454,7 +2472,7 @@
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="H3" s="3" t="n"/>
@@ -2497,7 +2515,7 @@
       </c>
       <c r="G4" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="H4" s="3" t="n"/>
@@ -2540,7 +2558,7 @@
       </c>
       <c r="G5" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="H5" s="3" t="n"/>
@@ -2670,7 +2688,7 @@
           <t>24/03/2025</t>
         </is>
       </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -2703,7 +2721,7 @@
           <t>Herlem Carlen Ferro</t>
         </is>
       </c>
-      <c r="E3" s="6" t="inlineStr">
+      <c r="E3" s="7" t="inlineStr">
         <is>
           <t>Duplicado</t>
         </is>
@@ -2713,7 +2731,7 @@
           <t>06/03/2025, 06/03/2025</t>
         </is>
       </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -2756,7 +2774,7 @@
           <t>09/04/2025</t>
         </is>
       </c>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -2803,7 +2821,7 @@
           <t>07/03/2025</t>
         </is>
       </c>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -2823,283 +2841,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
-    <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="32" customWidth="1" min="4" max="4"/>
-    <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="27" customWidth="1" min="7" max="7"/>
-    <col width="87" customWidth="1" min="8" max="8"/>
-    <col width="34" customWidth="1" min="9" max="9"/>
-    <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="26" customWidth="1" min="11" max="11"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Regional</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Município</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>UVR</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Técnico de UVR</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Situação</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Data de Envio</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Validado pelo Regional</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Observações</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Formulários para Deletar (ID)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Validado Equip de TI</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Resposta Equipe de TI</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>Ana Luiza de Araujo e Silva</t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
-        <is>
-          <t>10/04/2025</t>
-        </is>
-      </c>
-      <c r="G2" s="5" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="H2" s="3" t="inlineStr">
-        <is>
-          <t>Corrigido pela técnica regional em 14/04 - Aguardando devolutiva da técnica de UVR</t>
-        </is>
-      </c>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" s="3" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K2" s="3" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>Herlem Carlen Ferro</t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>09/04/2025</t>
-        </is>
-      </c>
-      <c r="G3" s="5" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>Corrigido pela técnica regional em 14/04 - Aguardando devolutiva da técnica de UVR</t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="n"/>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K3" s="3" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>Monica Goreth Costa Ribeiro</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>15/04/2025</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="H4" s="3" t="inlineStr">
-        <is>
-          <t>Corrigido pela técnica regional em 14/04 - Aguardando devolutiva da técnica de UVR</t>
-        </is>
-      </c>
-      <c r="I4" s="3" t="n"/>
-      <c r="J4" s="3" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K4" s="3" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>Thiago da Sailva Santos</t>
-        </is>
-      </c>
-      <c r="E5" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>09/04/2025</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="H5" s="3" t="inlineStr">
-        <is>
-          <t>Corrigido pela técnica regional em 14/04 - Aguardando devolutiva do técnico de UVR</t>
-        </is>
-      </c>
-      <c r="I5" s="3" t="n"/>
-      <c r="J5" s="3" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K5" s="3" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3209,15 +2950,19 @@
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>12/05/2025</t>
+          <t>10/04/2025</t>
         </is>
       </c>
       <c r="G2" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="H2" s="3" t="n"/>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>Corrigido</t>
+        </is>
+      </c>
       <c r="I2" s="3" t="n"/>
       <c r="J2" s="3" t="inlineStr">
         <is>
@@ -3252,15 +2997,19 @@
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>10/05/2025</t>
+          <t>09/04/2025</t>
         </is>
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="H3" s="3" t="n"/>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>Corrigido</t>
+        </is>
+      </c>
       <c r="I3" s="3" t="n"/>
       <c r="J3" s="3" t="inlineStr">
         <is>
@@ -3295,15 +3044,304 @@
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
+          <t>15/04/2025</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>Corrigido</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>ID4643</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>Deletado 4643</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Ana Paula</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Belém</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>Thiago da Sailva Santos</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>09/04/2025</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>Corrigido</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="n"/>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="32" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="27" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="34" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="26" customWidth="1" min="11" max="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Município</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>UVR</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Técnico de UVR</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Situação</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Data de Envio</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Validado pelo Regional</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Observações</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Formulários para Deletar (ID)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Validado Equip de TI</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Resposta Equipe de TI</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Ana Paula</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Belém</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>Ana Luiza de Araujo e Silva</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>12/05/2025</t>
+        </is>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>Corrigido</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="n"/>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K2" s="3" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Ana Paula</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Belém</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>Herlem Carlen Ferro</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
           <t>10/05/2025</t>
         </is>
       </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>Corrigido</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="n"/>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Ana Paula</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Belém</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>Monica Goreth Costa Ribeiro</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>10/05/2025</t>
+        </is>
+      </c>
       <c r="G4" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="H4" s="3" t="n"/>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>Corrigido</t>
+        </is>
+      </c>
       <c r="I4" s="3" t="n"/>
       <c r="J4" s="3" t="inlineStr">
         <is>
@@ -3343,10 +3381,14 @@
       </c>
       <c r="G5" s="5" t="inlineStr">
         <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="H5" s="3" t="n"/>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>Formulário apto</t>
+        </is>
+      </c>
       <c r="I5" s="3" t="n"/>
       <c r="J5" s="3" t="inlineStr">
         <is>
@@ -3463,9 +3505,13 @@
           <t>Ana Luiza de Araujo e Silva</t>
         </is>
       </c>
-      <c r="E2" s="3" t="n"/>
+      <c r="E2" s="8" t="inlineStr">
+        <is>
+          <t>Atrasado</t>
+        </is>
+      </c>
       <c r="F2" s="3" t="n"/>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -3498,9 +3544,17 @@
           <t>Herlem Carlen Ferro</t>
         </is>
       </c>
-      <c r="E3" s="3" t="n"/>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>10/06/2025</t>
+        </is>
+      </c>
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -3533,9 +3587,17 @@
           <t>Monica Goreth Costa Ribeiro</t>
         </is>
       </c>
-      <c r="E4" s="3" t="n"/>
-      <c r="F4" s="3" t="n"/>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>12/06/2025</t>
+        </is>
+      </c>
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -3568,9 +3630,17 @@
           <t>Thiago da Sailva Santos</t>
         </is>
       </c>
-      <c r="E5" s="3" t="n"/>
-      <c r="F5" s="3" t="n"/>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>06/06/2025</t>
+        </is>
+      </c>
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -3694,7 +3764,7 @@
       </c>
       <c r="E2" s="3" t="n"/>
       <c r="F2" s="3" t="n"/>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -3729,7 +3799,7 @@
       </c>
       <c r="E3" s="3" t="n"/>
       <c r="F3" s="3" t="n"/>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -3764,7 +3834,7 @@
       </c>
       <c r="E4" s="3" t="n"/>
       <c r="F4" s="3" t="n"/>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -3799,7 +3869,7 @@
       </c>
       <c r="E5" s="3" t="n"/>
       <c r="F5" s="3" t="n"/>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -3923,7 +3993,7 @@
       </c>
       <c r="E2" s="3" t="n"/>
       <c r="F2" s="3" t="n"/>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -3958,7 +4028,7 @@
       </c>
       <c r="E3" s="3" t="n"/>
       <c r="F3" s="3" t="n"/>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -3993,7 +4063,7 @@
       </c>
       <c r="E4" s="3" t="n"/>
       <c r="F4" s="3" t="n"/>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -4028,7 +4098,7 @@
       </c>
       <c r="E5" s="3" t="n"/>
       <c r="F5" s="3" t="n"/>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>

</xml_diff>